<commit_message>
added "other" instead of NaN in the ghgrp to include all unit type
</commit_message>
<xml_diff>
--- a/generic_heat_repartition/data/325193_process_parameters.xlsx
+++ b/generic_heat_repartition/data/325193_process_parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aidan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antoine\Documents\GitHub\Industrial-decarb\generic_heat_repartition\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C49ABDC-AD9E-4BB9-BCE2-AE60BA7E6CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A502E330-10DF-476F-865B-2270F7269A3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{0642930E-F94A-4C66-BE8E-0DAB4CA0F57B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{0642930E-F94A-4C66-BE8E-0DAB4CA0F57B}"/>
   </bookViews>
   <sheets>
     <sheet name="unit heat demand" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>Unit name</t>
   </si>
@@ -636,10 +636,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDFE9A88-4F80-4F9A-BB30-87A4EF6ABDB3}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -650,7 +650,7 @@
     <col min="4" max="4" width="24.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -664,7 +664,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -675,7 +675,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -686,7 +686,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -700,7 +700,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -711,7 +711,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -722,9 +722,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G14">
-        <v>4</v>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -736,7 +742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E4F7D68-99EF-4AA7-94B6-0E4B3576F10F}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>

</xml_diff>